<commit_message>
Alterações e refinamentos de casos de uso
Alterações e refinamentos dos casos de uso.
</commit_message>
<xml_diff>
--- a/casos de testes/Casos de testes - RecTourist.xlsx
+++ b/casos de testes/Casos de testes - RecTourist.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Capa" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Cadastro de usuário" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Cadastro de ponto turístico" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Planilha4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Pesquisar Pontos Turísticos" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -93,31 +93,377 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Preencher os campos </t>
+    </r>
+    <r>
+      <rPr>
         <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t>Nome, Sobrenome, Endereço, E-mail, Senha, Confirmar Senha e Sexo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> do usuário corretamente e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Confirma.</t>
+    </r>
+  </si>
+  <si>
+    <t>O ator terá cadastrado um usuário na aplicação RecTourist e estará logado na aplicação.</t>
+  </si>
+  <si>
+    <t>NÂO TESTADO</t>
+  </si>
+  <si>
+    <t>'FA-CT002</t>
+  </si>
+  <si>
+    <t>Cadastrar usuário com e-mail inválido</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Preencher o campo</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> E-mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> usuário com informações incorretas e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Confirma.</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema apresentará uma mensagem de erro para o usuário informando que o e-mail não é válido</t>
+  </si>
+  <si>
+    <t>'FA-CT003</t>
+  </si>
+  <si>
+    <t>Cadastrar usuário já existente</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Preencher o campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>e-mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> usuário já existentes e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Confirma.</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema apresentará uma mensagem de erro para o usuário informando que o e-mail já está cadastrado</t>
+  </si>
+  <si>
+    <t>'FA-CT004</t>
+  </si>
+  <si>
+    <t>Cadastrar usuário sem preencher todos os campos</t>
+  </si>
+  <si>
+    <t>Não preencher algum campo solicitado no momento do cadastro</t>
+  </si>
+  <si>
+    <t>O sistema apresentará uma mensagem de erro para o usuário informando existem campos não preenchidos e especificando qual campo está faltando</t>
+  </si>
+  <si>
+    <t>Tela Principal &gt; Cadastros de Pontos Turísticos</t>
+  </si>
+  <si>
+    <t>Testar a funcionalidade de incluir pontos turísticos no sistema RecTourist</t>
+  </si>
+  <si>
+    <t>Tela de Acesso ao sistema </t>
+  </si>
+  <si>
+    <t>Ter um administrador cadastrado no sistema</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Preencher os campos </t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Nome, Sobrenome, Endereço, E-mail, Senha, Confirmar Senha e Sexo</t>
-    </r>
-    <r>
-      <rPr>
         <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t>Nome do Usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> e </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Senha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> do administrador corretamente e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Acessar.</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema será carregado para a tela principal do RecTourist</t>
+  </si>
+  <si>
+    <t>Cadastrar Ponto Turístico</t>
+  </si>
+  <si>
+    <t>Ter um administrador logado no sistema</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Preencher o campo</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> Nome, Endereço e Descrição </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>do Ponto Turístico com as informações corretas clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Confirma.</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema apresentará uma mensagem de Ponto turístico cadastrado com sucesso</t>
+  </si>
+  <si>
+    <t>Cadastrar Ponto Turístico sem preencher todos os campos</t>
+  </si>
+  <si>
+    <t>Cadastrar Ponto turístico já existente</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Preencher os campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Nome ou Endereço </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>do ponto turístico já existentes e clicar em </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Confirma.</t>
+    </r>
+  </si>
+  <si>
+    <t>O sistema apresentará uma mensagem de erro para o usuário informando que o ponto turístico está cadastrado</t>
+  </si>
+  <si>
+    <t>Tela Principal &gt; Pesquisar Pontos Turísticos</t>
+  </si>
+  <si>
+    <t>Usuário estar logado no sistema e existirem pontos turísticos previamente cadastrados</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Preencher os campos </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Nome do Usuário</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t> e </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Senha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t> do usuário corretamente e clicar em </t>
     </r>
     <r>
@@ -127,484 +473,39 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Confirma</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>O ator terá cadastrado um usuário na aplicação RecTourist e estará logado na aplicação.</t>
-  </si>
-  <si>
-    <t>NÂO TESTADO</t>
-  </si>
-  <si>
-    <t>'FA-CT002</t>
-  </si>
-  <si>
-    <t>Cadastrar usuário com e-mail inválido</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Preencher o campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> E-mail</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> usuário com informações incorretas e clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Confirma</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema apresentará uma mensagem de erro para o usuário informando que o e-mail não é válido</t>
-  </si>
-  <si>
-    <t>'FA-CT003</t>
-  </si>
-  <si>
-    <t>Cadastrar usuário já existente</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Preencher o campo </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>e-mail</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> usuário já existentes e clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Confirma</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema apresentará uma mensagem de erro para o usuário informando que o e-mail já está cadastrado</t>
-  </si>
-  <si>
-    <t>'FA-CT004</t>
-  </si>
-  <si>
-    <t>Cadastrar usuário sem preencher todos os campos</t>
-  </si>
-  <si>
-    <t>Não preencher algum campo solicitado no momento do cadastro</t>
-  </si>
-  <si>
-    <t>O sistema apresentará uma mensagem de erro para o usuário informando existem campos não preenchidos e especificando qual campo está faltando</t>
-  </si>
-  <si>
-    <t>Tela Principal &gt; Cadastros de Pontos Turísticos</t>
-  </si>
-  <si>
-    <t>Testar a funcionalidade de incluir pontos turísticos no sistema RecTourist</t>
-  </si>
-  <si>
-    <t>Tela de Acesso ao sistema </t>
-  </si>
-  <si>
-    <t>Ter um administrador cadastrado no sistema</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Preencher os campos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Nome do Usuário</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> e </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Senha</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> do administrador corretamente e clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Acessar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema será carregado para a tela principal do RecTourist</t>
-  </si>
-  <si>
-    <t>Cadastrar Ponto Turístico</t>
-  </si>
-  <si>
-    <t>Ter um administrador logado no sistema</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Preencher o campo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> Nome, Endereço e Descrição </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>do Ponto Turístico com as informações corretas clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Confirma</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema apresentará uma mensagem de Ponto turístico cadastrado com sucesso</t>
-  </si>
-  <si>
-    <t>Cadastrar Ponto Turístico sem preencher todos os campos</t>
-  </si>
-  <si>
-    <t>Cadastrar Ponto turístico já existente</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Preencher os campo </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Nome ou Endereço </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>do ponto turístico já existentes e clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Confirma</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema apresentará uma mensagem de erro para o usuário informando que o ponto turístico está cadastrado</t>
-  </si>
-  <si>
-    <t>Tela Principal &gt; Pesquisar Pontos Turísticos</t>
-  </si>
-  <si>
-    <t>Usuário estar logado no sistema e existirem pontos turísticos previamente cadastrados</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Preencher os campos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Nome do Usuário</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> e </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Senha</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> do usuário corretamente e clicar em </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Acessar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
+      <t>Acessar.</t>
     </r>
   </si>
   <si>
     <t>Pesquisar Pontos Turísticos</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>O usuário insere sua localização atual e clica no botão </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+    <t>O usuário insere sua localização atual e clica no botão Pesquisar.</t>
+  </si>
+  <si>
+    <t>O sistema apresentará ao usuário um mapa contendo os pontos turísticos mais próximos e o usuário selecionará o ponto turístico de sua preferência.</t>
+  </si>
+  <si>
+    <t>Pesquisar Pontos Turísticos não existentes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Após inserir a posição atual o usuário clica no botão </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t>Pesquisar.</t>
-    </r>
-  </si>
-  <si>
-    <t>O sistema apresentará ao usuário um mapa contendo os pontos turísticos mais próximos e o usuário selecionará o ponto turístico de sua preferência.</t>
-  </si>
-  <si>
-    <t>Pesquisar Pontos Turísticos não existentes</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Após inserir a posição atual o usuário clica no botão </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Pesquisar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
     </r>
   </si>
   <si>
@@ -620,11 +521,12 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;CT&quot;000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -640,12 +542,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="20"/>
@@ -941,12 +837,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -991,26 +887,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1039,79 +935,87 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="21" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="21" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="22" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="22" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="23" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="23" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="24" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="24" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="7" borderId="25" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="25" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="26" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="26" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1123,7 +1027,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1201,7 +1105,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,17 +1511,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.1836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1772,20 +1676,20 @@
       <c r="C10" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="39" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
       <c r="M10" s="26" t="s">
         <v>24</v>
       </c>
@@ -1808,20 +1712,20 @@
       <c r="C12" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
       <c r="M12" s="26" t="s">
         <v>24</v>
       </c>
@@ -1835,7 +1739,7 @@
       <c r="A13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="38" t="s">
@@ -1844,20 +1748,20 @@
       <c r="C14" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
       <c r="M14" s="26" t="s">
         <v>24</v>
       </c>
@@ -1868,7 +1772,7 @@
       <c r="R14" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="43" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="38" t="s">
@@ -1883,14 +1787,14 @@
       <c r="E16" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
       <c r="M16" s="26" t="s">
         <v>24</v>
       </c>
@@ -1924,7 +1828,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -1945,17 +1849,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.1836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2110,20 +2014,20 @@
       <c r="C10" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
       <c r="M10" s="26" t="s">
         <v>24</v>
       </c>
@@ -2146,20 +2050,20 @@
       <c r="C12" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
       <c r="M12" s="26" t="s">
         <v>24</v>
       </c>
@@ -2173,7 +2077,7 @@
       <c r="A13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="38" t="s">
@@ -2188,14 +2092,14 @@
       <c r="E14" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
       <c r="M14" s="26" t="s">
         <v>24</v>
       </c>
@@ -2206,7 +2110,7 @@
       <c r="R14" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="43" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="38" t="s">
@@ -2215,20 +2119,20 @@
       <c r="C16" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
       <c r="M16" s="26" t="s">
         <v>24</v>
       </c>
@@ -2262,7 +2166,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -2278,22 +2182,22 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.1836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2448,20 +2352,20 @@
       <c r="C10" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="39" t="s">
         <v>53</v>
       </c>
       <c r="E10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
       <c r="M10" s="26" t="s">
         <v>24</v>
       </c>
@@ -2484,20 +2388,20 @@
       <c r="C12" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="39" t="s">
         <v>55</v>
       </c>
       <c r="E12" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
       <c r="M12" s="26" t="s">
         <v>24</v>
       </c>
@@ -2511,7 +2415,7 @@
       <c r="A13" s="36"/>
     </row>
     <row r="14" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="38" t="s">
@@ -2520,20 +2424,20 @@
       <c r="C14" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="39" t="s">
         <v>58</v>
       </c>
       <c r="E14" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
       <c r="M14" s="26" t="s">
         <v>24</v>
       </c>
@@ -2567,7 +2471,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>